<commit_message>
Mod: Optimized cat_script.sh and modified README.md directory structure.
</commit_message>
<xml_diff>
--- a/docs/aedes_genomes_specs/Ae_genomes_info.xlsx
+++ b/docs/aedes_genomes_specs/Ae_genomes_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10222"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Parsimony/Desktop/jorge_folder/Info/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Parsimony/GitHub_Projects/mosquito_virome_yucatan_LEVE/docs/aedes_genomes_specs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E973CFD3-3247-E04C-861D-E51C3C4F1EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2450AF5D-6536-EC40-BFEA-355712F9C476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20580" yWindow="820" windowWidth="20560" windowHeight="24300" xr2:uid="{3BF1FBAB-C882-E246-910D-7BE330E812F5}"/>
+    <workbookView xWindow="20560" yWindow="800" windowWidth="20560" windowHeight="24300" xr2:uid="{3BF1FBAB-C882-E246-910D-7BE330E812F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Ae_genomes_info" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
   <si>
     <t>taxon_id</t>
   </si>
@@ -179,6 +179,9 @@
   </si>
   <si>
     <t>source_link</t>
+  </si>
+  <si>
+    <t>NOT DOWNLOADED</t>
   </si>
 </sst>
 </file>
@@ -677,10 +680,11 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1059,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F921960-DEBB-8F44-9FA7-F6235BBD9038}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1068,6 +1072,10 @@
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="3" max="4" width="24.83203125" customWidth="1"/>
     <col min="5" max="5" width="16.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -1142,7 +1150,10 @@
       <c r="J2">
         <v>3</v>
       </c>
-      <c r="L2" t="s">
+      <c r="K2" s="3">
+        <v>46079</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>28</v>
       </c>
       <c r="M2" t="s">
@@ -1180,7 +1191,10 @@
       <c r="J3">
         <v>3</v>
       </c>
-      <c r="L3" t="s">
+      <c r="K3" s="3">
+        <v>46079</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>31</v>
       </c>
       <c r="M3" t="s">
@@ -1218,7 +1232,9 @@
       <c r="J4" s="1">
         <v>3</v>
       </c>
-      <c r="K4" s="1"/>
+      <c r="K4" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="L4" s="1" t="s">
         <v>32</v>
       </c>
@@ -1257,7 +1273,10 @@
       <c r="J5">
         <v>3</v>
       </c>
-      <c r="L5" t="s">
+      <c r="K5" s="3">
+        <v>46079</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>36</v>
       </c>
       <c r="M5" t="s">
@@ -1295,7 +1314,10 @@
       <c r="J6">
         <v>3</v>
       </c>
-      <c r="L6" t="s">
+      <c r="K6" s="3">
+        <v>46079</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>39</v>
       </c>
       <c r="M6" t="s">
@@ -1333,6 +1355,9 @@
       <c r="J7">
         <v>3</v>
       </c>
+      <c r="K7" s="3">
+        <v>46079</v>
+      </c>
       <c r="L7" s="2" t="s">
         <v>41</v>
       </c>
@@ -1371,7 +1396,10 @@
       <c r="J8">
         <v>3</v>
       </c>
-      <c r="L8" t="s">
+      <c r="K8" s="3">
+        <v>46079</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="M8" t="s">
@@ -1409,7 +1437,10 @@
       <c r="J9">
         <v>3</v>
       </c>
-      <c r="L9" t="s">
+      <c r="K9" s="3">
+        <v>46079</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>25</v>
       </c>
       <c r="M9" t="s">
@@ -1419,6 +1450,12 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L7" r:id="rId1" xr:uid="{B16F3449-581F-6C48-8115-FDFD92085D4D}"/>
+    <hyperlink ref="L2" r:id="rId2" xr:uid="{4AE2B16C-682F-DD4E-A649-9F588167DAFF}"/>
+    <hyperlink ref="L3" r:id="rId3" xr:uid="{83245D94-34D5-674F-88E3-EDF3BD3778D4}"/>
+    <hyperlink ref="L5" r:id="rId4" xr:uid="{53AD2075-4F55-7744-B464-19B3EF3D77F6}"/>
+    <hyperlink ref="L6" r:id="rId5" xr:uid="{EBD1DBFC-718D-B443-9310-A28E3AE588EB}"/>
+    <hyperlink ref="L8" r:id="rId6" xr:uid="{F9672871-9B6F-7644-A0DB-E823E208FF90}"/>
+    <hyperlink ref="L9" r:id="rId7" xr:uid="{516B9BBA-B9AB-1F4E-95DC-BB39C6D42D21}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>